<commit_message>
Working on results for LH regional
glmmpql broken with lsmeans? trying to get stargazer to work but doesn't like class of glmmpql
</commit_message>
<xml_diff>
--- a/lifehist/Life hist site clim.xlsx
+++ b/lifehist/Life hist site clim.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Biome</t>
   </si>
   <si>
-    <t>Average mean temp (min, max)</t>
-  </si>
-  <si>
-    <t>Ecoregion (State)</t>
-  </si>
-  <si>
     <t>Latitude (group)</t>
   </si>
   <si>
@@ -45,9 +39,6 @@
     <t>28.6 (25.6, 33.2)</t>
   </si>
   <si>
-    <t>Imeri (Amazonas)</t>
-  </si>
-  <si>
     <t>-2.864 (1)</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>26.4 (23.1, 31.9)</t>
   </si>
   <si>
-    <t>Madeira (Rondonia)</t>
-  </si>
-  <si>
     <t>-8.742 (2)</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t>28.4 (23.3, 35.4)</t>
   </si>
   <si>
-    <t>Cerrado (Tocantins)</t>
-  </si>
-  <si>
     <t>-10.7 (2)</t>
   </si>
   <si>
@@ -114,13 +99,28 @@
     <t>21.4 (17, 27.8)</t>
   </si>
   <si>
-    <t>Atlantic (Rio de Janeiro)</t>
-  </si>
-  <si>
     <t>-22.611 (3)</t>
   </si>
   <si>
     <t>SJU</t>
+  </si>
+  <si>
+    <t>Average mean temp (min, max) *</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Amazonas</t>
+  </si>
+  <si>
+    <t>Rondonia</t>
+  </si>
+  <si>
+    <t>Tocantins</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -720,6 +720,32 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -776,7 +802,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -789,35 +815,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -826,6 +825,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1198,33 +1233,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="3"/>
-      <c r="H1" s="18"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="1">
         <v>20</v>
       </c>
@@ -1236,20 +1271,20 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>145</v>
@@ -1262,18 +1297,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="23"/>
       <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>218</v>
@@ -1286,18 +1319,18 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="F5" s="1">
         <v>219</v>
@@ -1310,18 +1343,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>20</v>
+      <c r="E6" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="1">
         <v>223</v>
@@ -1334,20 +1365,20 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
+      <c r="A7" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="F7" s="1">
         <v>120</v>
@@ -1360,18 +1391,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="1">
         <v>59</v>
@@ -1384,20 +1413,20 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>29</v>
+      <c r="A9" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="F9" s="6">
         <v>160</v>
@@ -1410,14 +1439,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>